<commit_message>
Updated Acceptance Test Plan.xlsx to have all Product back log stories
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Tremblay\Desktop\Computer Science Course Work\swen261\etc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0A8DB2-4789-4701-9636-8849D8E77D8C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4320" windowWidth="18705" windowHeight="7545" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -55,18 +61,6 @@
     <t>Given that the player I selected is already in a game when I select that player then the system will return me to the Home page with an error message.</t>
   </si>
   <si>
-    <t>Given a valid, initial game board when I drag a piece to a white space then the piece should not be droppable.</t>
-  </si>
-  <si>
-    <t>Given a valid, initial game board when I drag a piece to an occupied space then the piece should not be droppable.</t>
-  </si>
-  <si>
-    <t>Given a valid, initial game board when I drag a piece to an open space then the piece should be droppable.  NOTE: In this Story the drop action should not do anything; piece movement will be the focus of future stories.</t>
-  </si>
-  <si>
-    <t>Given a valid, initial game board when I view the board in the browser then my pieces are oriented on the bottom of the board grid just like I would see the board if I were playing in the physical world.</t>
-  </si>
-  <si>
     <t>As a Player I want to sign-in so that I can play a game of checkers.</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>Given that no one else is using my name when I enter my name containing at least one alphanumeric character and optionally spaces in the sign-in form and click the Sign-in button then I expect the system to reserve my name and navigate back to the Home page.</t>
   </si>
   <si>
-    <t>Given that I am not signed-in when I do click on the sign-in link then I expect to be taken to the Sign-in page, with a means to enter a player name.</t>
-  </si>
-  <si>
     <t>Given that I am on the Sign-in page when I enter a name that does not contain at least one alphanumeric character or contains one or more characters that are not alphanumeric or spaces and click the Sign-in button then I expect the system to reject this name and return the Sign-in page.</t>
   </si>
   <si>
@@ -112,11 +103,26 @@
   <si>
     <t>Given that I'm waiting for a game when another player selects a game with me then the system will automatically send me to the Game View as the White player.  NOTE: the `home.ftl` HTML includes a `&lt;meta&gt;` tag that tells the browser to refresh the game every 5 seconds; thus you need to update the `GetHomeRoute` controller to handle the situation when a player is assigned a game.</t>
   </si>
+  <si>
+    <t>Given that I am not signed-in when I do click on the sign-in link then I expect to be taken to the Sign-in page with a means to enter a player name.</t>
+  </si>
+  <si>
+    <t>Given a valid initial game board when I drag a piece to a white space then the piece should not be droppable.</t>
+  </si>
+  <si>
+    <t>Given a valid initial game board when I drag a piece to an occupied space then the piece should not be droppable.</t>
+  </si>
+  <si>
+    <t>Given a valid initial game board when I drag a piece to an open space then the piece should be droppable.  NOTE: In this Story the drop action should not do anything; piece movement will be the focus of future stories.</t>
+  </si>
+  <si>
+    <t>Given a valid initial game board when I view the board in the browser then my pieces are oriented on the bottom of the board grid just like I would see the board if I were playing in the physical world.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -256,6 +262,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -582,7 +591,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -600,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -608,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -616,7 +625,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +639,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H597"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -659,27 +668,27 @@
         <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -691,7 +700,7 @@
     <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="8"/>
       <c r="E3" s="8"/>
@@ -700,7 +709,7 @@
     <row r="4" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" s="8"/>
       <c r="E4" s="8"/>
@@ -709,7 +718,7 @@
     <row r="5" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C5" s="8"/>
       <c r="E5" s="8"/>
@@ -718,7 +727,7 @@
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C6" s="8"/>
       <c r="E6" s="8"/>
@@ -744,7 +753,7 @@
     </row>
     <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>8</v>
@@ -777,7 +786,7 @@
     <row r="12" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C12" s="8"/>
       <c r="E12" s="8"/>
@@ -786,7 +795,7 @@
     <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C13" s="8"/>
       <c r="E13" s="8"/>
@@ -795,7 +804,7 @@
     <row r="14" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C14" s="8"/>
       <c r="E14" s="8"/>
@@ -804,7 +813,7 @@
     <row r="15" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C15" s="8"/>
       <c r="E15" s="8"/>
@@ -813,7 +822,7 @@
     <row r="16" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C16" s="8"/>
       <c r="E16" s="8"/>
@@ -3744,7 +3753,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E597 C2:C597 G2:G597">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E597 C2:C597 G2:G597" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>